<commit_message>
Add graph units for elapsed time
</commit_message>
<xml_diff>
--- a/L2/compiled-data.xlsx
+++ b/L2/compiled-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/GitHub/CS3210-Labs/L2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341847FE-F904-AD46-B0FE-275E72C4D5F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F006566-2BBF-A049-9882-2E044F827396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16280" activeTab="1" xr2:uid="{0FBFC964-02DC-EF4A-BC51-50E6BD43A8BE}"/>
   </bookViews>
@@ -16,12 +16,12 @@
     <sheet name="i7-7700" sheetId="1" r:id="rId1"/>
     <sheet name="xs-4114" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId3"/>
-    <pivotCache cacheId="18" r:id="rId4"/>
-    <pivotCache cacheId="25" r:id="rId5"/>
-    <pivotCache cacheId="37" r:id="rId6"/>
+    <pivotCache cacheId="39" r:id="rId3"/>
+    <pivotCache cacheId="40" r:id="rId4"/>
+    <pivotCache cacheId="41" r:id="rId5"/>
+    <pivotCache cacheId="42" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -160,14 +160,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -315,6 +314,15 @@
               <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
+          <c:showLegendKey val="1"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="1"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
@@ -343,7 +351,7 @@
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="10"/>
+        <c:idx val="2"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -368,7 +376,7 @@
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="11"/>
+        <c:idx val="3"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -393,7 +401,7 @@
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="12"/>
+        <c:idx val="4"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -418,7 +426,7 @@
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="13"/>
+        <c:idx val="5"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -443,7 +451,7 @@
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="14"/>
+        <c:idx val="6"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -468,8 +476,11 @@
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="15"/>
+        <c:idx val="7"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -493,7 +504,7 @@
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="16"/>
+        <c:idx val="8"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -518,8 +529,11 @@
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="17"/>
+        <c:idx val="9"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -543,8 +557,11 @@
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="18"/>
+        <c:idx val="10"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -597,11 +614,23 @@
               <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
+          <c:showLegendKey val="1"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="1"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="19"/>
+        <c:idx val="11"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -654,10 +683,285 @@
               <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
+          <c:showLegendKey val="1"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="1"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="20"/>
+        <c:idx val="12"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="13"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="14"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="15"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="16"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="17"/>
         <c:spPr>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
@@ -713,7 +1017,37 @@
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="21"/>
+        <c:idx val="18"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="19"/>
         <c:spPr>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
@@ -757,228 +1091,6 @@
               <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="27"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="28"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="29"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="30"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="31"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1602,6 +1714,9 @@
       <c:pivotFmt>
         <c:idx val="0"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1714,6 +1829,9 @@
       <c:pivotFmt>
         <c:idx val="2"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1741,6 +1859,9 @@
       <c:pivotFmt>
         <c:idx val="3"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1768,6 +1889,9 @@
       <c:pivotFmt>
         <c:idx val="4"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1780,6 +1904,9 @@
       <c:pivotFmt>
         <c:idx val="5"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1788,6 +1915,62 @@
           </a:ln>
           <a:effectLst/>
         </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
@@ -3193,7 +3376,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-GB"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4026,7 +4209,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-GB"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4804,7 +4987,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-GB"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5698,6 +5881,9 @@
       <c:pivotFmt>
         <c:idx val="2"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -5754,6 +5940,9 @@
       <c:pivotFmt>
         <c:idx val="3"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -6315,6 +6504,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -6527,6 +6771,9 @@
       <c:pivotFmt>
         <c:idx val="0"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -6583,6 +6830,9 @@
       <c:pivotFmt>
         <c:idx val="1"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -7356,6 +7606,9 @@
       <c:pivotFmt>
         <c:idx val="0"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -7412,6 +7665,9 @@
       <c:pivotFmt>
         <c:idx val="1"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -7468,6 +7724,9 @@
       <c:pivotFmt>
         <c:idx val="2"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -7523,6 +7782,121 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
         <c:spPr>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
@@ -19348,7 +19722,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B32C658C-0C7A-3245-84C7-79374EF1A9A7}" name="PivotTable4" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B32C658C-0C7A-3245-84C7-79374EF1A9A7}" name="PivotTable4" cacheId="40" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="K45:N61" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField axis="axisCol" showAll="0">
@@ -19500,7 +19874,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{46B60E4B-6734-4042-AB3C-7F8EF597AB06}" name="PivotTable3" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{46B60E4B-6734-4042-AB3C-7F8EF597AB06}" name="PivotTable3" cacheId="39" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="K25:N41" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisCol" showAll="0">
@@ -19612,7 +19986,7 @@
   <dataFields count="1">
     <dataField name="Average of cyclesPerInstruction" fld="7" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="6">
+  <chartFormats count="7">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -19694,6 +20068,18 @@
         </references>
       </pivotArea>
     </chartFormat>
+    <chartFormat chart="0" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -19708,7 +20094,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{17DFA615-9157-154B-94AA-1A210D94E4B7}" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{17DFA615-9157-154B-94AA-1A210D94E4B7}" name="PivotTable1" cacheId="39" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13">
   <location ref="K5:N21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisCol" showAll="0">
@@ -19820,56 +20206,8 @@
   <dataFields count="1">
     <dataField name="Average of timeElapsed" fld="6" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="7">
-    <chartFormat chart="0" format="6" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="27" series="1">
+  <chartFormats count="4">
+    <chartFormat chart="0" format="14" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -19878,7 +20216,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="28" series="1">
+    <chartFormat chart="0" format="15" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -19887,7 +20225,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="30" series="1">
+    <chartFormat chart="0" format="17" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -19895,6 +20233,18 @@
           </reference>
           <reference field="0" count="1" selected="0">
             <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="19" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
@@ -19913,7 +20263,158 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{04588326-0C20-A646-A455-72A6C0F801DA}" name="PivotTable10" cacheId="37" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0C443F9A-5C7F-4746-AE16-6632F08BF2B7}" name="PivotTable5" cacheId="41" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
+  <location ref="K2:N18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="15">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="15">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of timeElapsed" fld="5" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="3">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{04588326-0C20-A646-A455-72A6C0F801DA}" name="PivotTable10" cacheId="42" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14">
   <location ref="K101:N117" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField axis="axisCol" showAll="0">
@@ -20028,7 +20529,7 @@
   <dataFields count="1">
     <dataField name="Average of MFLOPS" fld="8" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="4">
+  <chartFormats count="6">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -20065,6 +20566,30 @@
         </references>
       </pivotArea>
     </chartFormat>
+    <chartFormat chart="6" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -20078,8 +20603,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8D7BAD6-9A0A-C64E-BA7A-321BB3818177}" name="PivotTable9" cacheId="37" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14">
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8D7BAD6-9A0A-C64E-BA7A-321BB3818177}" name="PivotTable9" cacheId="42" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14">
   <location ref="K80:N96" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField axis="axisCol" showAll="0">
@@ -20322,8 +20847,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{395234E2-4247-F342-969A-7E59F6C39179}" name="PivotTable8" cacheId="37" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{395234E2-4247-F342-969A-7E59F6C39179}" name="PivotTable8" cacheId="42" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14">
   <location ref="K59:N75" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField axis="axisCol" showAll="0">
@@ -20518,8 +21043,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BF7C5A6E-0979-A54A-B980-BBD9B75ECEFE}" name="PivotTable7" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BF7C5A6E-0979-A54A-B980-BBD9B75ECEFE}" name="PivotTable7" cacheId="41" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="K38:N54" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisCol" showAll="0">
@@ -20669,8 +21194,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F68105BA-2581-1B44-B6F5-D73EA1C2DF1B}" name="PivotTable6" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F68105BA-2581-1B44-B6F5-D73EA1C2DF1B}" name="PivotTable6" cacheId="41" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="K20:N36" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisCol" showAll="0">
@@ -20772,157 +21297,6 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Average of IPC" fld="6" subtotal="average" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="3">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0C443F9A-5C7F-4746-AE16-6632F08BF2B7}" name="PivotTable5" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
-  <location ref="K2:N18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="8">
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="15">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="15">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="0"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of timeElapsed" fld="5" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <chartFormats count="3">
     <chartFormat chart="0" format="0" series="1">
@@ -21554,13 +21928,13 @@
       <c r="K7" s="3">
         <v>1</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7">
         <v>6.1667908613333333</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7">
         <v>9.1020401936666655</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7">
         <v>7.6344155274999999</v>
       </c>
     </row>
@@ -21597,13 +21971,13 @@
       <c r="K8" s="3">
         <v>2</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8">
         <v>3.0183461503333331</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M8">
         <v>4.7393932956666669</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N8">
         <v>3.8788697229999998</v>
       </c>
     </row>
@@ -21640,13 +22014,13 @@
       <c r="K9" s="3">
         <v>4</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9">
         <v>1.5883661</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9">
         <v>2.5285954610000001</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9">
         <v>2.0584807805000001</v>
       </c>
     </row>
@@ -21683,13 +22057,13 @@
       <c r="K10" s="3">
         <v>8</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10">
         <v>1.6814443603333331</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10">
         <v>1.3563629193333331</v>
       </c>
-      <c r="N10" s="4">
+      <c r="N10">
         <v>1.5189036398333331</v>
       </c>
     </row>
@@ -21726,13 +22100,13 @@
       <c r="K11" s="3">
         <v>16</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11">
         <v>1.812451005</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11">
         <v>1.3171784500000001</v>
       </c>
-      <c r="N11" s="4">
+      <c r="N11">
         <v>1.5648147274999999</v>
       </c>
     </row>
@@ -21769,13 +22143,13 @@
       <c r="K12" s="3">
         <v>32</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12">
         <v>2.1593609136666667</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12">
         <v>1.150457641</v>
       </c>
-      <c r="N12" s="4">
+      <c r="N12">
         <v>1.6549092773333332</v>
       </c>
     </row>
@@ -21812,13 +22186,13 @@
       <c r="K13" s="3">
         <v>64</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13">
         <v>1.7197387196666665</v>
       </c>
-      <c r="M13" s="4">
+      <c r="M13">
         <v>1.1064692893333334</v>
       </c>
-      <c r="N13" s="4">
+      <c r="N13">
         <v>1.4131040045000001</v>
       </c>
     </row>
@@ -21855,13 +22229,13 @@
       <c r="K14" s="3">
         <v>128</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14">
         <v>1.6922543030000001</v>
       </c>
-      <c r="M14" s="4">
+      <c r="M14">
         <v>1.0946780783333334</v>
       </c>
-      <c r="N14" s="4">
+      <c r="N14">
         <v>1.3934661906666668</v>
       </c>
     </row>
@@ -21898,13 +22272,13 @@
       <c r="K15" s="3">
         <v>256</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15">
         <v>1.6705698353333334</v>
       </c>
-      <c r="M15" s="4">
+      <c r="M15">
         <v>1.0860770123333332</v>
       </c>
-      <c r="N15" s="4">
+      <c r="N15">
         <v>1.3783234238333335</v>
       </c>
     </row>
@@ -21941,13 +22315,13 @@
       <c r="K16" s="3">
         <v>512</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16">
         <v>1.7849111879999999</v>
       </c>
-      <c r="M16" s="4">
+      <c r="M16">
         <v>1.1019053343333334</v>
       </c>
-      <c r="N16" s="4">
+      <c r="N16">
         <v>1.4434082611666668</v>
       </c>
     </row>
@@ -21984,13 +22358,13 @@
       <c r="K17" s="3">
         <v>1024</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17">
         <v>2.1511113003333331</v>
       </c>
-      <c r="M17" s="4">
+      <c r="M17">
         <v>1.1124290773333332</v>
       </c>
-      <c r="N17" s="4">
+      <c r="N17">
         <v>1.6317701888333331</v>
       </c>
     </row>
@@ -22027,13 +22401,13 @@
       <c r="K18" s="3">
         <v>2048</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18">
         <v>1.827385623666667</v>
       </c>
-      <c r="M18" s="4">
+      <c r="M18">
         <v>1.1509589603333332</v>
       </c>
-      <c r="N18" s="4">
+      <c r="N18">
         <v>1.4891722920000001</v>
       </c>
     </row>
@@ -22070,13 +22444,13 @@
       <c r="K19" s="3">
         <v>4096</v>
       </c>
-      <c r="L19" s="4">
+      <c r="L19">
         <v>1.7462536786666665</v>
       </c>
-      <c r="M19" s="4">
+      <c r="M19">
         <v>1.2378259206666666</v>
       </c>
-      <c r="N19" s="4">
+      <c r="N19">
         <v>1.4920397996666666</v>
       </c>
     </row>
@@ -22113,13 +22487,13 @@
       <c r="K20" s="3">
         <v>8192</v>
       </c>
-      <c r="L20" s="4">
+      <c r="L20">
         <v>1.8346160303333334</v>
       </c>
-      <c r="M20" s="4">
+      <c r="M20">
         <v>1.4035760990000001</v>
       </c>
-      <c r="N20" s="4">
+      <c r="N20">
         <v>1.6190960646666666</v>
       </c>
     </row>
@@ -22156,13 +22530,13 @@
       <c r="K21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L21" s="4">
+      <c r="L21">
         <v>2.2038285764047623</v>
       </c>
-      <c r="M21" s="4">
+      <c r="M21">
         <v>2.1062819808809525</v>
       </c>
-      <c r="N21" s="4">
+      <c r="N21">
         <v>2.1550552786428576</v>
       </c>
     </row>
@@ -22378,13 +22752,13 @@
       <c r="K27" s="3">
         <v>1</v>
       </c>
-      <c r="L27" s="4">
+      <c r="L27">
         <v>2.4076769468528578</v>
       </c>
-      <c r="M27" s="4">
+      <c r="M27">
         <v>2.2278394772788119</v>
       </c>
-      <c r="N27" s="4">
+      <c r="N27">
         <v>2.3177582120658351</v>
       </c>
     </row>
@@ -22421,13 +22795,13 @@
       <c r="K28" s="3">
         <v>2</v>
       </c>
-      <c r="L28" s="4">
+      <c r="L28">
         <v>2.4157323407162026</v>
       </c>
-      <c r="M28" s="4">
+      <c r="M28">
         <v>2.220824222621351</v>
       </c>
-      <c r="N28" s="4">
+      <c r="N28">
         <v>2.3182782816687766</v>
       </c>
     </row>
@@ -22464,13 +22838,13 @@
       <c r="K29" s="3">
         <v>4</v>
       </c>
-      <c r="L29" s="4">
+      <c r="L29">
         <v>2.3790139511671304</v>
       </c>
-      <c r="M29" s="4">
+      <c r="M29">
         <v>2.21280815178776</v>
       </c>
-      <c r="N29" s="4">
+      <c r="N29">
         <v>2.2959110514774452</v>
       </c>
     </row>
@@ -22507,13 +22881,13 @@
       <c r="K30" s="3">
         <v>8</v>
       </c>
-      <c r="L30" s="4">
+      <c r="L30">
         <v>1.1558801447832747</v>
       </c>
-      <c r="M30" s="4">
+      <c r="M30">
         <v>2.1943161759558136</v>
       </c>
-      <c r="N30" s="4">
+      <c r="N30">
         <v>1.6750981603695443</v>
       </c>
     </row>
@@ -22550,13 +22924,13 @@
       <c r="K31" s="3">
         <v>16</v>
       </c>
-      <c r="L31" s="4">
+      <c r="L31">
         <v>1.1695089138302655</v>
       </c>
-      <c r="M31" s="4">
+      <c r="M31">
         <v>1.390976938696934</v>
       </c>
-      <c r="N31" s="4">
+      <c r="N31">
         <v>1.2802429262635997</v>
       </c>
     </row>
@@ -22593,13 +22967,13 @@
       <c r="K32" s="3">
         <v>32</v>
       </c>
-      <c r="L32" s="4">
+      <c r="L32">
         <v>1.155469148515321</v>
       </c>
-      <c r="M32" s="4">
+      <c r="M32">
         <v>1.2256246183089632</v>
       </c>
-      <c r="N32" s="4">
+      <c r="N32">
         <v>1.1905468834121422</v>
       </c>
     </row>
@@ -22636,13 +23010,13 @@
       <c r="K33" s="3">
         <v>64</v>
       </c>
-      <c r="L33" s="4">
+      <c r="L33">
         <v>1.1591265117003167</v>
       </c>
-      <c r="M33" s="4">
+      <c r="M33">
         <v>1.2166504370382578</v>
       </c>
-      <c r="N33" s="4">
+      <c r="N33">
         <v>1.1878884743692875</v>
       </c>
     </row>
@@ -22679,13 +23053,13 @@
       <c r="K34" s="3">
         <v>128</v>
       </c>
-      <c r="L34" s="4">
+      <c r="L34">
         <v>1.1583606842822549</v>
       </c>
-      <c r="M34" s="4">
+      <c r="M34">
         <v>1.2109437932680469</v>
       </c>
-      <c r="N34" s="4">
+      <c r="N34">
         <v>1.1846522387751508</v>
       </c>
     </row>
@@ -22722,13 +23096,13 @@
       <c r="K35" s="3">
         <v>256</v>
       </c>
-      <c r="L35" s="4">
+      <c r="L35">
         <v>1.1656314787265984</v>
       </c>
-      <c r="M35" s="4">
+      <c r="M35">
         <v>1.2157992514626306</v>
       </c>
-      <c r="N35" s="4">
+      <c r="N35">
         <v>1.1907153650946145</v>
       </c>
     </row>
@@ -22765,13 +23139,13 @@
       <c r="K36" s="3">
         <v>512</v>
       </c>
-      <c r="L36" s="4">
+      <c r="L36">
         <v>1.176442518889689</v>
       </c>
-      <c r="M36" s="4">
+      <c r="M36">
         <v>1.2094115245345636</v>
       </c>
-      <c r="N36" s="4">
+      <c r="N36">
         <v>1.1929270217121262</v>
       </c>
     </row>
@@ -22808,13 +23182,13 @@
       <c r="K37" s="3">
         <v>1024</v>
       </c>
-      <c r="L37" s="4">
+      <c r="L37">
         <v>1.1795559668196092</v>
       </c>
-      <c r="M37" s="4">
+      <c r="M37">
         <v>1.2204459738307125</v>
       </c>
-      <c r="N37" s="4">
+      <c r="N37">
         <v>1.2000009703251606</v>
       </c>
     </row>
@@ -22851,13 +23225,13 @@
       <c r="K38" s="3">
         <v>2048</v>
       </c>
-      <c r="L38" s="4">
+      <c r="L38">
         <v>1.1847030461034902</v>
       </c>
-      <c r="M38" s="4">
+      <c r="M38">
         <v>1.2160389457423848</v>
       </c>
-      <c r="N38" s="4">
+      <c r="N38">
         <v>1.2003709959229374</v>
       </c>
     </row>
@@ -22894,13 +23268,13 @@
       <c r="K39" s="3">
         <v>4096</v>
       </c>
-      <c r="L39" s="4">
+      <c r="L39">
         <v>1.1788333565888311</v>
       </c>
-      <c r="M39" s="4">
+      <c r="M39">
         <v>1.2003900898255571</v>
       </c>
-      <c r="N39" s="4">
+      <c r="N39">
         <v>1.1896117232071941</v>
       </c>
     </row>
@@ -22937,13 +23311,13 @@
       <c r="K40" s="3">
         <v>8192</v>
       </c>
-      <c r="L40" s="4">
+      <c r="L40">
         <v>1.1753004272162091</v>
       </c>
-      <c r="M40" s="4">
+      <c r="M40">
         <v>1.1683905976432374</v>
       </c>
-      <c r="N40" s="4">
+      <c r="N40">
         <v>1.1718455124297231</v>
       </c>
     </row>
@@ -22980,13 +23354,13 @@
       <c r="K41" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L41" s="4">
+      <c r="L41">
         <v>1.4329453882994319</v>
       </c>
-      <c r="M41" s="4">
+      <c r="M41">
         <v>1.5093185855710731</v>
       </c>
-      <c r="N41" s="4">
+      <c r="N41">
         <v>1.4711319869352526</v>
       </c>
     </row>
@@ -23202,13 +23576,13 @@
       <c r="K47" s="3">
         <v>1</v>
       </c>
-      <c r="L47" s="4">
+      <c r="L47">
         <v>9609.2054591139859</v>
       </c>
-      <c r="M47" s="4">
+      <c r="M47">
         <v>6506.4010007346251</v>
       </c>
-      <c r="N47" s="4">
+      <c r="N47">
         <v>8057.8032299243059</v>
       </c>
     </row>
@@ -23245,13 +23619,13 @@
       <c r="K48" s="3">
         <v>2</v>
       </c>
-      <c r="L48" s="4">
+      <c r="L48">
         <v>19622.404204608316</v>
       </c>
-      <c r="M48" s="4">
+      <c r="M48">
         <v>12496.530843266586</v>
       </c>
-      <c r="N48" s="4">
+      <c r="N48">
         <v>16059.46752393745</v>
       </c>
     </row>
@@ -23288,13 +23662,13 @@
       <c r="K49" s="3">
         <v>4</v>
       </c>
-      <c r="L49" s="4">
+      <c r="L49">
         <v>37289.816414581408</v>
       </c>
-      <c r="M49" s="4">
+      <c r="M49">
         <v>23428.557962531911</v>
       </c>
-      <c r="N49" s="4">
+      <c r="N49">
         <v>30359.187188556662</v>
       </c>
     </row>
@@ -23331,13 +23705,13 @@
       <c r="K50" s="3">
         <v>8</v>
       </c>
-      <c r="L50" s="4">
+      <c r="L50">
         <v>35250.759177422951</v>
       </c>
-      <c r="M50" s="4">
+      <c r="M50">
         <v>43683.461907137527</v>
       </c>
-      <c r="N50" s="4">
+      <c r="N50">
         <v>39467.110542280243</v>
       </c>
     </row>
@@ -23374,13 +23748,13 @@
       <c r="K51" s="3">
         <v>16</v>
       </c>
-      <c r="L51" s="4">
+      <c r="L51">
         <v>32691.288716395957</v>
       </c>
-      <c r="M51" s="4">
+      <c r="M51">
         <v>45021.854712264147</v>
       </c>
-      <c r="N51" s="4">
+      <c r="N51">
         <v>38856.57171433005</v>
       </c>
     </row>
@@ -23417,13 +23791,13 @@
       <c r="K52" s="3">
         <v>32</v>
       </c>
-      <c r="L52" s="4">
+      <c r="L52">
         <v>27556.055065491422</v>
       </c>
-      <c r="M52" s="4">
+      <c r="M52">
         <v>51498.794096145721</v>
       </c>
-      <c r="N52" s="4">
+      <c r="N52">
         <v>39527.424580818573</v>
       </c>
     </row>
@@ -23460,13 +23834,13 @@
       <c r="K53" s="3">
         <v>64</v>
       </c>
-      <c r="L53" s="4">
+      <c r="L53">
         <v>34455.42304716535</v>
       </c>
-      <c r="M53" s="4">
+      <c r="M53">
         <v>53556.736286741274</v>
       </c>
-      <c r="N53" s="4">
+      <c r="N53">
         <v>44006.079666953308</v>
       </c>
     </row>
@@ -23503,13 +23877,13 @@
       <c r="K54" s="3">
         <v>128</v>
       </c>
-      <c r="L54" s="4">
+      <c r="L54">
         <v>35022.395948736892</v>
       </c>
-      <c r="M54" s="4">
+      <c r="M54">
         <v>54154.645154807979</v>
       </c>
-      <c r="N54" s="4">
+      <c r="N54">
         <v>44588.520551772439</v>
       </c>
     </row>
@@ -23546,13 +23920,13 @@
       <c r="K55" s="3">
         <v>256</v>
       </c>
-      <c r="L55" s="4">
+      <c r="L55">
         <v>35493.387554301451</v>
       </c>
-      <c r="M55" s="4">
+      <c r="M55">
         <v>54590.596308502754</v>
       </c>
-      <c r="N55" s="4">
+      <c r="N55">
         <v>45041.991931402103</v>
       </c>
     </row>
@@ -23589,13 +23963,13 @@
       <c r="K56" s="3">
         <v>512</v>
       </c>
-      <c r="L56" s="4">
+      <c r="L56">
         <v>33263.612876323306</v>
       </c>
-      <c r="M56" s="4">
+      <c r="M56">
         <v>53840.598248385744</v>
       </c>
-      <c r="N56" s="4">
+      <c r="N56">
         <v>43552.105562354525</v>
       </c>
     </row>
@@ -23632,13 +24006,13 @@
       <c r="K57" s="3">
         <v>1024</v>
       </c>
-      <c r="L57" s="4">
+      <c r="L57">
         <v>27634.146716638905</v>
       </c>
-      <c r="M57" s="4">
+      <c r="M57">
         <v>53389.025321542606</v>
       </c>
-      <c r="N57" s="4">
+      <c r="N57">
         <v>40511.586019090755</v>
       </c>
     </row>
@@ -23675,13 +24049,13 @@
       <c r="K58" s="3">
         <v>2048</v>
       </c>
-      <c r="L58" s="4">
+      <c r="L58">
         <v>33054.225003196108</v>
       </c>
-      <c r="M58" s="4">
+      <c r="M58">
         <v>51714.044886430202</v>
       </c>
-      <c r="N58" s="4">
+      <c r="N58">
         <v>42384.134944813151</v>
       </c>
     </row>
@@ -23718,13 +24092,13 @@
       <c r="K59" s="3">
         <v>4096</v>
       </c>
-      <c r="L59" s="4">
+      <c r="L59">
         <v>34238.858320742329</v>
       </c>
-      <c r="M59" s="4">
+      <c r="M59">
         <v>48291.942482839921</v>
       </c>
-      <c r="N59" s="4">
+      <c r="N59">
         <v>41265.400401791128</v>
       </c>
     </row>
@@ -23761,13 +24135,13 @@
       <c r="K60" s="3">
         <v>8192</v>
       </c>
-      <c r="L60" s="4">
+      <c r="L60">
         <v>32870.422790952034</v>
       </c>
-      <c r="M60" s="4">
+      <c r="M60">
         <v>42955.572667843247</v>
       </c>
-      <c r="N60" s="4">
+      <c r="N60">
         <v>37912.997729397648</v>
       </c>
     </row>
@@ -23804,13 +24178,13 @@
       <c r="K61" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L61" s="4">
+      <c r="L61">
         <v>30575.142949690737</v>
       </c>
-      <c r="M61" s="4">
+      <c r="M61">
         <v>42509.197277083869</v>
       </c>
-      <c r="N61" s="4">
+      <c r="N61">
         <v>36542.170113387314</v>
       </c>
     </row>
@@ -27173,8 +27547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{190DE68E-6C45-2C40-9EF8-7A7DDED5B4C0}">
   <dimension ref="A1:N127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G68" zoomScale="75" workbookViewId="0">
-      <selection activeCell="S96" sqref="S96"/>
+    <sheetView tabSelected="1" topLeftCell="F31" zoomScale="75" workbookViewId="0">
+      <selection activeCell="U59" sqref="U59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27333,13 +27707,13 @@
       <c r="K4" s="3">
         <v>1</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4">
         <v>5.2112511043333329</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4">
         <v>6.3068850099999993</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4">
         <v>5.7590680571666661</v>
       </c>
     </row>
@@ -27376,13 +27750,13 @@
       <c r="K5" s="3">
         <v>2</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5">
         <v>2.6618961873333333</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5">
         <v>3.3443314726666671</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5">
         <v>3.0031138300000002</v>
       </c>
     </row>
@@ -27419,13 +27793,13 @@
       <c r="K6" s="3">
         <v>4</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6">
         <v>1.4370475213333334</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6">
         <v>1.8741973950000002</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6">
         <v>1.6556224581666665</v>
       </c>
     </row>
@@ -27462,13 +27836,13 @@
       <c r="K7" s="3">
         <v>8</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7">
         <v>3.1226173126666672</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7">
         <v>1.0277483813333335</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7">
         <v>2.0751828470000007</v>
       </c>
     </row>
@@ -27505,13 +27879,13 @@
       <c r="K8" s="3">
         <v>16</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8">
         <v>3.1662040516666665</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M8">
         <v>1.522962022</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N8">
         <v>2.3445830368333334</v>
       </c>
     </row>
@@ -27548,13 +27922,13 @@
       <c r="K9" s="3">
         <v>32</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9">
         <v>3.2223494013333336</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9">
         <v>2.0946923230000003</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9">
         <v>2.6585208621666667</v>
       </c>
     </row>
@@ -27591,13 +27965,13 @@
       <c r="K10" s="3">
         <v>64</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10">
         <v>3.3288154063333337</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10">
         <v>2.0566337303333331</v>
       </c>
-      <c r="N10" s="4">
+      <c r="N10">
         <v>2.6927245683333338</v>
       </c>
     </row>
@@ -27634,13 +28008,13 @@
       <c r="K11" s="3">
         <v>128</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11">
         <v>3.2006867106666665</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11">
         <v>2.0528761416666668</v>
       </c>
-      <c r="N11" s="4">
+      <c r="N11">
         <v>2.6267814261666662</v>
       </c>
     </row>
@@ -27677,13 +28051,13 @@
       <c r="K12" s="3">
         <v>256</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12">
         <v>3.150042531</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12">
         <v>2.0814839219999999</v>
       </c>
-      <c r="N12" s="4">
+      <c r="N12">
         <v>2.6157632264999999</v>
       </c>
     </row>
@@ -27720,13 +28094,13 @@
       <c r="K13" s="3">
         <v>512</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13">
         <v>3.528577683</v>
       </c>
-      <c r="M13" s="4">
+      <c r="M13">
         <v>2.0681213409999999</v>
       </c>
-      <c r="N13" s="4">
+      <c r="N13">
         <v>2.7983495120000001</v>
       </c>
     </row>
@@ -27763,13 +28137,13 @@
       <c r="K14" s="3">
         <v>1024</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14">
         <v>3.0987979549999998</v>
       </c>
-      <c r="M14" s="4">
+      <c r="M14">
         <v>2.0876795476666667</v>
       </c>
-      <c r="N14" s="4">
+      <c r="N14">
         <v>2.5932387513333333</v>
       </c>
     </row>
@@ -27806,13 +28180,13 @@
       <c r="K15" s="3">
         <v>2048</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15">
         <v>3.3733782906666665</v>
       </c>
-      <c r="M15" s="4">
+      <c r="M15">
         <v>2.1136502789999998</v>
       </c>
-      <c r="N15" s="4">
+      <c r="N15">
         <v>2.7435142848333332</v>
       </c>
     </row>
@@ -27849,13 +28223,13 @@
       <c r="K16" s="3">
         <v>4096</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16">
         <v>3.2420289256666668</v>
       </c>
-      <c r="M16" s="4">
+      <c r="M16">
         <v>2.1916656446666667</v>
       </c>
-      <c r="N16" s="4">
+      <c r="N16">
         <v>2.7168472851666667</v>
       </c>
     </row>
@@ -27892,13 +28266,13 @@
       <c r="K17" s="3">
         <v>8192</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17">
         <v>3.3744578089999995</v>
       </c>
-      <c r="M17" s="4">
+      <c r="M17">
         <v>2.3953863070000003</v>
       </c>
-      <c r="N17" s="4">
+      <c r="N17">
         <v>2.8849220579999995</v>
       </c>
     </row>
@@ -27935,13 +28309,13 @@
       <c r="K18" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18">
         <v>3.2227250635714277</v>
       </c>
-      <c r="M18" s="4">
+      <c r="M18">
         <v>2.372736679809524</v>
       </c>
-      <c r="N18" s="4">
+      <c r="N18">
         <v>2.7977308716904759</v>
       </c>
     </row>
@@ -28089,13 +28463,13 @@
       <c r="K22" s="3">
         <v>1</v>
       </c>
-      <c r="L22" s="4">
+      <c r="L22">
         <v>1.2707020867048886</v>
       </c>
-      <c r="M22" s="4">
+      <c r="M22">
         <v>1.4886891141714056</v>
       </c>
-      <c r="N22" s="4">
+      <c r="N22">
         <v>1.3796956004381471</v>
       </c>
     </row>
@@ -28132,13 +28506,13 @@
       <c r="K23" s="3">
         <v>2</v>
       </c>
-      <c r="L23" s="4">
+      <c r="L23">
         <v>1.2778753527318598</v>
       </c>
-      <c r="M23" s="4">
+      <c r="M23">
         <v>1.4733999210670674</v>
       </c>
-      <c r="N23" s="4">
+      <c r="N23">
         <v>1.3756376368994638</v>
       </c>
     </row>
@@ -28175,13 +28549,13 @@
       <c r="K24" s="3">
         <v>4</v>
       </c>
-      <c r="L24" s="4">
+      <c r="L24">
         <v>1.2460825419389836</v>
       </c>
-      <c r="M24" s="4">
+      <c r="M24">
         <v>1.4292522054281829</v>
       </c>
-      <c r="N24" s="4">
+      <c r="N24">
         <v>1.3376673736835833</v>
       </c>
     </row>
@@ -28218,13 +28592,13 @@
       <c r="K25" s="3">
         <v>8</v>
       </c>
-      <c r="L25" s="4">
+      <c r="L25">
         <v>0.28634754933859963</v>
       </c>
-      <c r="M25" s="4">
+      <c r="M25">
         <v>1.4551137544771533</v>
       </c>
-      <c r="N25" s="4">
+      <c r="N25">
         <v>0.87073065190787646</v>
       </c>
     </row>
@@ -28261,13 +28635,13 @@
       <c r="K26" s="3">
         <v>16</v>
       </c>
-      <c r="L26" s="4">
+      <c r="L26">
         <v>0.28802338893565144</v>
       </c>
-      <c r="M26" s="4">
+      <c r="M26">
         <v>0.66663182235879692</v>
       </c>
-      <c r="N26" s="4">
+      <c r="N26">
         <v>0.47732760564722421</v>
       </c>
     </row>
@@ -28304,13 +28678,13 @@
       <c r="K27" s="3">
         <v>32</v>
       </c>
-      <c r="L27" s="4">
+      <c r="L27">
         <v>0.28539884426625023</v>
       </c>
-      <c r="M27" s="4">
+      <c r="M27">
         <v>0.29994092592726923</v>
       </c>
-      <c r="N27" s="4">
+      <c r="N27">
         <v>0.29266988509675973</v>
       </c>
     </row>
@@ -28347,13 +28721,13 @@
       <c r="K28" s="3">
         <v>64</v>
       </c>
-      <c r="L28" s="4">
+      <c r="L28">
         <v>0.28622276850580453</v>
       </c>
-      <c r="M28" s="4">
+      <c r="M28">
         <v>0.29635403422631762</v>
       </c>
-      <c r="N28" s="4">
+      <c r="N28">
         <v>0.2912884013660611</v>
       </c>
     </row>
@@ -28390,13 +28764,13 @@
       <c r="K29" s="3">
         <v>128</v>
       </c>
-      <c r="L29" s="4">
+      <c r="L29">
         <v>0.28566942248861654</v>
       </c>
-      <c r="M29" s="4">
+      <c r="M29">
         <v>0.29284045089418326</v>
       </c>
-      <c r="N29" s="4">
+      <c r="N29">
         <v>0.2892549366913999</v>
       </c>
     </row>
@@ -28433,13 +28807,13 @@
       <c r="K30" s="3">
         <v>256</v>
       </c>
-      <c r="L30" s="4">
+      <c r="L30">
         <v>0.28603309332970112</v>
       </c>
-      <c r="M30" s="4">
+      <c r="M30">
         <v>0.29244047612934659</v>
       </c>
-      <c r="N30" s="4">
+      <c r="N30">
         <v>0.28923678472952385</v>
       </c>
     </row>
@@ -28476,13 +28850,13 @@
       <c r="K31" s="3">
         <v>512</v>
       </c>
-      <c r="L31" s="4">
+      <c r="L31">
         <v>0.28860211542351039</v>
       </c>
-      <c r="M31" s="4">
+      <c r="M31">
         <v>0.29342070966879169</v>
       </c>
-      <c r="N31" s="4">
+      <c r="N31">
         <v>0.29101141254615098</v>
       </c>
     </row>
@@ -28519,13 +28893,13 @@
       <c r="K32" s="3">
         <v>1024</v>
       </c>
-      <c r="L32" s="4">
+      <c r="L32">
         <v>0.29045695570180979</v>
       </c>
-      <c r="M32" s="4">
+      <c r="M32">
         <v>0.29323817097270694</v>
       </c>
-      <c r="N32" s="4">
+      <c r="N32">
         <v>0.29184756333725836</v>
       </c>
     </row>
@@ -28562,13 +28936,13 @@
       <c r="K33" s="3">
         <v>2048</v>
       </c>
-      <c r="L33" s="4">
+      <c r="L33">
         <v>0.29241562420736289</v>
       </c>
-      <c r="M33" s="4">
+      <c r="M33">
         <v>0.29450879173717831</v>
       </c>
-      <c r="N33" s="4">
+      <c r="N33">
         <v>0.29346220797227057</v>
       </c>
     </row>
@@ -28605,13 +28979,13 @@
       <c r="K34" s="3">
         <v>4096</v>
       </c>
-      <c r="L34" s="4">
+      <c r="L34">
         <v>0.29354803018850267</v>
       </c>
-      <c r="M34" s="4">
+      <c r="M34">
         <v>0.29403541014853457</v>
       </c>
-      <c r="N34" s="4">
+      <c r="N34">
         <v>0.29379172016851868</v>
       </c>
     </row>
@@ -28648,13 +29022,13 @@
       <c r="K35" s="3">
         <v>8192</v>
       </c>
-      <c r="L35" s="4">
+      <c r="L35">
         <v>0.29443434570343902</v>
       </c>
-      <c r="M35" s="4">
+      <c r="M35">
         <v>0.29186218020265314</v>
       </c>
-      <c r="N35" s="4">
+      <c r="N35">
         <v>0.29314826295304608</v>
       </c>
     </row>
@@ -28691,13 +29065,13 @@
       <c r="K36" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L36" s="4">
+      <c r="L36">
         <v>0.49798657996178425</v>
       </c>
-      <c r="M36" s="4">
+      <c r="M36">
         <v>0.65440914052925636</v>
       </c>
-      <c r="N36" s="4">
+      <c r="N36">
         <v>0.57619786024552022</v>
       </c>
     </row>
@@ -28845,13 +29219,13 @@
       <c r="K40" s="3">
         <v>1</v>
       </c>
-      <c r="L40" s="4">
+      <c r="L40">
         <v>1295.8571882403548</v>
       </c>
-      <c r="M40" s="4">
+      <c r="M40">
         <v>1070.261473884965</v>
       </c>
-      <c r="N40" s="4">
+      <c r="N40">
         <v>1183.05933106266</v>
       </c>
     </row>
@@ -28888,13 +29262,13 @@
       <c r="K41" s="3">
         <v>2</v>
       </c>
-      <c r="L41" s="4">
+      <c r="L41">
         <v>2536.1060803445525</v>
       </c>
-      <c r="M41" s="4">
+      <c r="M41">
         <v>2020.443218934307</v>
       </c>
-      <c r="N41" s="4">
+      <c r="N41">
         <v>2278.2746496394298</v>
       </c>
     </row>
@@ -28931,13 +29305,13 @@
       <c r="K42" s="3">
         <v>4</v>
       </c>
-      <c r="L42" s="4">
+      <c r="L42">
         <v>4699.2463502642795</v>
       </c>
-      <c r="M42" s="4">
+      <c r="M42">
         <v>3612.7404229612625</v>
       </c>
-      <c r="N42" s="4">
+      <c r="N42">
         <v>4155.9933866127712</v>
       </c>
     </row>
@@ -28974,13 +29348,13 @@
       <c r="K43" s="3">
         <v>8</v>
       </c>
-      <c r="L43" s="4">
+      <c r="L43">
         <v>2161.6718591373342</v>
       </c>
-      <c r="M43" s="4">
+      <c r="M43">
         <v>6568.6596826506357</v>
       </c>
-      <c r="N43" s="4">
+      <c r="N43">
         <v>4365.1657708939847</v>
       </c>
     </row>
@@ -29017,13 +29391,13 @@
       <c r="K44" s="3">
         <v>16</v>
       </c>
-      <c r="L44" s="4">
+      <c r="L44">
         <v>2131.9316389788864</v>
       </c>
-      <c r="M44" s="4">
+      <c r="M44">
         <v>4438.0232260862867</v>
       </c>
-      <c r="N44" s="4">
+      <c r="N44">
         <v>3284.9774325325866</v>
       </c>
     </row>
@@ -29060,13 +29434,13 @@
       <c r="K45" s="3">
         <v>32</v>
       </c>
-      <c r="L45" s="4">
+      <c r="L45">
         <v>2096.4439738507149</v>
       </c>
-      <c r="M45" s="4">
+      <c r="M45">
         <v>3223.2295946191352</v>
       </c>
-      <c r="N45" s="4">
+      <c r="N45">
         <v>2659.8367842349248</v>
       </c>
     </row>
@@ -29103,13 +29477,13 @@
       <c r="K46" s="3">
         <v>64</v>
       </c>
-      <c r="L46" s="4">
+      <c r="L46">
         <v>2027.7895074541066</v>
       </c>
-      <c r="M46" s="4">
+      <c r="M46">
         <v>3282.1927515595976</v>
       </c>
-      <c r="N46" s="4">
+      <c r="N46">
         <v>2654.9911295068518</v>
       </c>
     </row>
@@ -29146,13 +29520,13 @@
       <c r="K47" s="3">
         <v>128</v>
       </c>
-      <c r="L47" s="4">
+      <c r="L47">
         <v>2110.4217627260873</v>
       </c>
-      <c r="M47" s="4">
+      <c r="M47">
         <v>3288.163709660615</v>
       </c>
-      <c r="N47" s="4">
+      <c r="N47">
         <v>2699.2927361933507</v>
       </c>
     </row>
@@ -29189,13 +29563,13 @@
       <c r="K48" s="3">
         <v>256</v>
       </c>
-      <c r="L48" s="4">
+      <c r="L48">
         <v>2142.9916475377277</v>
       </c>
-      <c r="M48" s="4">
+      <c r="M48">
         <v>3243.0971845915738</v>
       </c>
-      <c r="N48" s="4">
+      <c r="N48">
         <v>2693.0444160646507</v>
       </c>
     </row>
@@ -29232,13 +29606,13 @@
       <c r="K49" s="3">
         <v>512</v>
       </c>
-      <c r="L49" s="4">
+      <c r="L49">
         <v>1919.8533007059359</v>
       </c>
-      <c r="M49" s="4">
+      <c r="M49">
         <v>3263.900874867662</v>
       </c>
-      <c r="N49" s="4">
+      <c r="N49">
         <v>2591.8770877867992</v>
       </c>
     </row>
@@ -29275,13 +29649,13 @@
       <c r="K50" s="3">
         <v>1024</v>
       </c>
-      <c r="L50" s="4">
+      <c r="L50">
         <v>2178.2977778294567</v>
       </c>
-      <c r="M50" s="4">
+      <c r="M50">
         <v>3233.272055196278</v>
       </c>
-      <c r="N50" s="4">
+      <c r="N50">
         <v>2705.7849165128669</v>
       </c>
     </row>
@@ -29318,13 +29692,13 @@
       <c r="K51" s="3">
         <v>2048</v>
       </c>
-      <c r="L51" s="4">
+      <c r="L51">
         <v>2012.2920646291075</v>
       </c>
-      <c r="M51" s="4">
+      <c r="M51">
         <v>3193.5390171177046</v>
       </c>
-      <c r="N51" s="4">
+      <c r="N51">
         <v>2602.9155408734059</v>
       </c>
     </row>
@@ -29361,13 +29735,13 @@
       <c r="K52" s="3">
         <v>4096</v>
       </c>
-      <c r="L52" s="4">
+      <c r="L52">
         <v>2083.9133291870789</v>
       </c>
-      <c r="M52" s="4">
+      <c r="M52">
         <v>3079.8622138927335</v>
       </c>
-      <c r="N52" s="4">
+      <c r="N52">
         <v>2581.8877715399062</v>
       </c>
     </row>
@@ -29404,13 +29778,13 @@
       <c r="K53" s="3">
         <v>8192</v>
       </c>
-      <c r="L53" s="4">
+      <c r="L53">
         <v>2001.1468335069949</v>
       </c>
-      <c r="M53" s="4">
+      <c r="M53">
         <v>2818.0683825461874</v>
       </c>
-      <c r="N53" s="4">
+      <c r="N53">
         <v>2409.6076080265912</v>
       </c>
     </row>
@@ -29447,13 +29821,13 @@
       <c r="K54" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L54" s="4">
+      <c r="L54">
         <v>2242.7116653137587</v>
       </c>
-      <c r="M54" s="4">
+      <c r="M54">
         <v>3309.6752720406394</v>
       </c>
-      <c r="N54" s="4">
+      <c r="N54">
         <v>2776.1934686771983</v>
       </c>
     </row>
@@ -29700,13 +30074,13 @@
       <c r="K61" s="3">
         <v>1</v>
       </c>
-      <c r="L61" s="4">
+      <c r="L61">
         <v>6.3068850099999993</v>
       </c>
-      <c r="M61" s="4">
+      <c r="M61">
         <v>4.7057995020000005</v>
       </c>
-      <c r="N61" s="4">
+      <c r="N61">
         <v>5.5063422559999999</v>
       </c>
     </row>
@@ -29743,13 +30117,13 @@
       <c r="K62" s="3">
         <v>2</v>
       </c>
-      <c r="L62" s="4">
+      <c r="L62">
         <v>3.3443314726666671</v>
       </c>
-      <c r="M62" s="4">
+      <c r="M62">
         <v>2.5126172216666665</v>
       </c>
-      <c r="N62" s="4">
+      <c r="N62">
         <v>2.9284743471666665</v>
       </c>
     </row>
@@ -29786,13 +30160,13 @@
       <c r="K63" s="3">
         <v>4</v>
       </c>
-      <c r="L63" s="4">
+      <c r="L63">
         <v>1.8741973950000002</v>
       </c>
-      <c r="M63" s="4">
+      <c r="M63">
         <v>1.3842280973333334</v>
       </c>
-      <c r="N63" s="4">
+      <c r="N63">
         <v>1.6292127461666668</v>
       </c>
     </row>
@@ -29829,13 +30203,13 @@
       <c r="K64" s="3">
         <v>8</v>
       </c>
-      <c r="L64" s="4">
+      <c r="L64">
         <v>1.0277483813333335</v>
       </c>
-      <c r="M64" s="4">
+      <c r="M64">
         <v>0.78875139300000008</v>
       </c>
-      <c r="N64" s="4">
+      <c r="N64">
         <v>0.90824988716666677</v>
       </c>
     </row>
@@ -29872,13 +30246,13 @@
       <c r="K65" s="3">
         <v>16</v>
       </c>
-      <c r="L65" s="4">
+      <c r="L65">
         <v>1.522962022</v>
       </c>
-      <c r="M65" s="4">
+      <c r="M65">
         <v>0.49503663733333331</v>
       </c>
-      <c r="N65" s="4">
+      <c r="N65">
         <v>1.0089993296666666</v>
       </c>
     </row>
@@ -29915,13 +30289,13 @@
       <c r="K66" s="3">
         <v>32</v>
       </c>
-      <c r="L66" s="4">
+      <c r="L66">
         <v>2.0946923230000003</v>
       </c>
-      <c r="M66" s="4">
+      <c r="M66">
         <v>0.44606583933333338</v>
       </c>
-      <c r="N66" s="4">
+      <c r="N66">
         <v>1.2703790811666666</v>
       </c>
     </row>
@@ -29958,13 +30332,13 @@
       <c r="K67" s="3">
         <v>64</v>
       </c>
-      <c r="L67" s="4">
+      <c r="L67">
         <v>2.0566337303333331</v>
       </c>
-      <c r="M67" s="4">
+      <c r="M67">
         <v>0.4334147963333333</v>
       </c>
-      <c r="N67" s="4">
+      <c r="N67">
         <v>1.2450242633333335</v>
       </c>
     </row>
@@ -30001,13 +30375,13 @@
       <c r="K68" s="3">
         <v>128</v>
       </c>
-      <c r="L68" s="4">
+      <c r="L68">
         <v>2.0528761416666668</v>
       </c>
-      <c r="M68" s="4">
+      <c r="M68">
         <v>0.43659658466666668</v>
       </c>
-      <c r="N68" s="4">
+      <c r="N68">
         <v>1.2447363631666668</v>
       </c>
     </row>
@@ -30044,13 +30418,13 @@
       <c r="K69" s="3">
         <v>256</v>
       </c>
-      <c r="L69" s="4">
+      <c r="L69">
         <v>2.0814839219999999</v>
       </c>
-      <c r="M69" s="4">
+      <c r="M69">
         <v>0.44530895199999998</v>
       </c>
-      <c r="N69" s="4">
+      <c r="N69">
         <v>1.2633964369999999</v>
       </c>
     </row>
@@ -30087,13 +30461,13 @@
       <c r="K70" s="3">
         <v>512</v>
       </c>
-      <c r="L70" s="4">
+      <c r="L70">
         <v>2.0681213409999999</v>
       </c>
-      <c r="M70" s="4">
+      <c r="M70">
         <v>0.45105376866666669</v>
       </c>
-      <c r="N70" s="4">
+      <c r="N70">
         <v>1.2595875548333335</v>
       </c>
     </row>
@@ -30130,13 +30504,13 @@
       <c r="K71" s="3">
         <v>1024</v>
       </c>
-      <c r="L71" s="4">
+      <c r="L71">
         <v>2.0876795476666667</v>
       </c>
-      <c r="M71" s="4">
+      <c r="M71">
         <v>0.47715491133333332</v>
       </c>
-      <c r="N71" s="4">
+      <c r="N71">
         <v>1.2824172294999998</v>
       </c>
     </row>
@@ -30173,13 +30547,13 @@
       <c r="K72" s="3">
         <v>2048</v>
       </c>
-      <c r="L72" s="4">
+      <c r="L72">
         <v>2.1136502789999998</v>
       </c>
-      <c r="M72" s="4">
+      <c r="M72">
         <v>0.51561414466666677</v>
       </c>
-      <c r="N72" s="4">
+      <c r="N72">
         <v>1.3146322118333331</v>
       </c>
     </row>
@@ -30216,13 +30590,13 @@
       <c r="K73" s="3">
         <v>4096</v>
       </c>
-      <c r="L73" s="4">
+      <c r="L73">
         <v>2.1916656446666667</v>
       </c>
-      <c r="M73" s="4">
+      <c r="M73">
         <v>0.59393427199999993</v>
       </c>
-      <c r="N73" s="4">
+      <c r="N73">
         <v>1.3927999583333335</v>
       </c>
     </row>
@@ -30259,13 +30633,13 @@
       <c r="K74" s="3">
         <v>8192</v>
       </c>
-      <c r="L74" s="4">
+      <c r="L74">
         <v>2.3953863070000003</v>
       </c>
-      <c r="M74" s="4">
+      <c r="M74">
         <v>0.75559478433333327</v>
       </c>
-      <c r="N74" s="4">
+      <c r="N74">
         <v>1.5754905456666668</v>
       </c>
     </row>
@@ -30302,13 +30676,13 @@
       <c r="K75" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L75" s="4">
+      <c r="L75">
         <v>2.372736679809524</v>
       </c>
-      <c r="M75" s="4">
+      <c r="M75">
         <v>1.03151220747619</v>
       </c>
-      <c r="N75" s="4">
+      <c r="N75">
         <v>1.7021244436428571</v>
       </c>
     </row>
@@ -30555,13 +30929,13 @@
       <c r="K82" s="3">
         <v>1</v>
       </c>
-      <c r="L82" s="4">
+      <c r="L82">
         <v>1.4886891141714056</v>
       </c>
-      <c r="M82" s="4">
+      <c r="M82">
         <v>1.7526604966284172</v>
       </c>
-      <c r="N82" s="4">
+      <c r="N82">
         <v>1.6206748053999114</v>
       </c>
     </row>
@@ -30598,13 +30972,13 @@
       <c r="K83" s="3">
         <v>2</v>
       </c>
-      <c r="L83" s="4">
+      <c r="L83">
         <v>1.4733999210670674</v>
       </c>
-      <c r="M83" s="4">
+      <c r="M83">
         <v>1.7389428620227376</v>
       </c>
-      <c r="N83" s="4">
+      <c r="N83">
         <v>1.6061713915449023</v>
       </c>
     </row>
@@ -30641,13 +31015,13 @@
       <c r="K84" s="3">
         <v>4</v>
       </c>
-      <c r="L84" s="4">
+      <c r="L84">
         <v>1.4292522054281829</v>
       </c>
-      <c r="M84" s="4">
+      <c r="M84">
         <v>1.7210728025081092</v>
       </c>
-      <c r="N84" s="4">
+      <c r="N84">
         <v>1.5751625039681461</v>
       </c>
     </row>
@@ -30684,13 +31058,13 @@
       <c r="K85" s="3">
         <v>8</v>
       </c>
-      <c r="L85" s="4">
+      <c r="L85">
         <v>1.4551137544771533</v>
       </c>
-      <c r="M85" s="4">
+      <c r="M85">
         <v>1.689254630638894</v>
       </c>
-      <c r="N85" s="4">
+      <c r="N85">
         <v>1.5721841925580236</v>
       </c>
     </row>
@@ -30727,13 +31101,13 @@
       <c r="K86" s="3">
         <v>16</v>
       </c>
-      <c r="L86" s="4">
+      <c r="L86">
         <v>0.66663182235879692</v>
       </c>
-      <c r="M86" s="4">
+      <c r="M86">
         <v>1.6016225640562745</v>
       </c>
-      <c r="N86" s="4">
+      <c r="N86">
         <v>1.1341271932075359</v>
       </c>
     </row>
@@ -30770,13 +31144,13 @@
       <c r="K87" s="3">
         <v>32</v>
       </c>
-      <c r="L87" s="4">
+      <c r="L87">
         <v>0.29994092592726923</v>
       </c>
-      <c r="M87" s="4">
+      <c r="M87">
         <v>1.6946626690410458</v>
       </c>
-      <c r="N87" s="4">
+      <c r="N87">
         <v>0.99730179748415748</v>
       </c>
     </row>
@@ -30813,13 +31187,13 @@
       <c r="K88" s="3">
         <v>64</v>
       </c>
-      <c r="L88" s="4">
+      <c r="L88">
         <v>0.29635403422631762</v>
       </c>
-      <c r="M88" s="4">
+      <c r="M88">
         <v>1.6908285137486612</v>
       </c>
-      <c r="N88" s="4">
+      <c r="N88">
         <v>0.99359127398748959</v>
       </c>
     </row>
@@ -30856,13 +31230,13 @@
       <c r="K89" s="3">
         <v>128</v>
       </c>
-      <c r="L89" s="4">
+      <c r="L89">
         <v>0.29284045089418326</v>
       </c>
-      <c r="M89" s="4">
+      <c r="M89">
         <v>1.6874852934264624</v>
       </c>
-      <c r="N89" s="4">
+      <c r="N89">
         <v>0.99016287216032295</v>
       </c>
     </row>
@@ -30899,13 +31273,13 @@
       <c r="K90" s="3">
         <v>256</v>
       </c>
-      <c r="L90" s="4">
+      <c r="L90">
         <v>0.29244047612934659</v>
       </c>
-      <c r="M90" s="4">
+      <c r="M90">
         <v>1.6821763008147448</v>
       </c>
-      <c r="N90" s="4">
+      <c r="N90">
         <v>0.98730838847204572</v>
       </c>
     </row>
@@ -30942,13 +31316,13 @@
       <c r="K91" s="3">
         <v>512</v>
       </c>
-      <c r="L91" s="4">
+      <c r="L91">
         <v>0.29342070966879169</v>
       </c>
-      <c r="M91" s="4">
+      <c r="M91">
         <v>1.6765604881383522</v>
       </c>
-      <c r="N91" s="4">
+      <c r="N91">
         <v>0.98499059890357199</v>
       </c>
     </row>
@@ -30985,13 +31359,13 @@
       <c r="K92" s="3">
         <v>1024</v>
       </c>
-      <c r="L92" s="4">
+      <c r="L92">
         <v>0.29323817097270694</v>
       </c>
-      <c r="M92" s="4">
+      <c r="M92">
         <v>1.6591935297536409</v>
       </c>
-      <c r="N92" s="4">
+      <c r="N92">
         <v>0.97621585036317393</v>
       </c>
     </row>
@@ -31028,13 +31402,13 @@
       <c r="K93" s="3">
         <v>2048</v>
       </c>
-      <c r="L93" s="4">
+      <c r="L93">
         <v>0.29450879173717831</v>
       </c>
-      <c r="M93" s="4">
+      <c r="M93">
         <v>1.6241140130003382</v>
       </c>
-      <c r="N93" s="4">
+      <c r="N93">
         <v>0.95931140236875823</v>
       </c>
     </row>
@@ -31071,13 +31445,13 @@
       <c r="K94" s="3">
         <v>4096</v>
       </c>
-      <c r="L94" s="4">
+      <c r="L94">
         <v>0.29403541014853457</v>
       </c>
-      <c r="M94" s="4">
+      <c r="M94">
         <v>1.567056674947046</v>
       </c>
-      <c r="N94" s="4">
+      <c r="N94">
         <v>0.93054604254779039</v>
       </c>
     </row>
@@ -31114,13 +31488,13 @@
       <c r="K95" s="3">
         <v>8192</v>
       </c>
-      <c r="L95" s="4">
+      <c r="L95">
         <v>0.29186218020265314</v>
       </c>
-      <c r="M95" s="4">
+      <c r="M95">
         <v>1.4599840270723528</v>
       </c>
-      <c r="N95" s="4">
+      <c r="N95">
         <v>0.87592310363750292</v>
       </c>
     </row>
@@ -31157,13 +31531,13 @@
       <c r="K96" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L96" s="4">
+      <c r="L96">
         <v>0.65440914052925636</v>
       </c>
-      <c r="M96" s="4">
+      <c r="M96">
         <v>1.6604010618426481</v>
       </c>
-      <c r="N96" s="4">
+      <c r="N96">
         <v>1.1574051011859523</v>
       </c>
     </row>
@@ -31410,13 +31784,13 @@
       <c r="K103" s="3">
         <v>1</v>
       </c>
-      <c r="L103" s="4">
+      <c r="L103">
         <v>1070.261473884965</v>
       </c>
-      <c r="M103" s="4">
+      <c r="M103">
         <v>1434.4044976909263</v>
       </c>
-      <c r="N103" s="4">
+      <c r="N103">
         <v>1252.332985787946</v>
       </c>
     </row>
@@ -31453,13 +31827,13 @@
       <c r="K104" s="3">
         <v>2</v>
       </c>
-      <c r="L104" s="4">
+      <c r="L104">
         <v>2020.443218934307</v>
       </c>
-      <c r="M104" s="4">
+      <c r="M104">
         <v>2686.5697708594967</v>
       </c>
-      <c r="N104" s="4">
+      <c r="N104">
         <v>2353.5064948969016</v>
       </c>
     </row>
@@ -31496,13 +31870,13 @@
       <c r="K105" s="3">
         <v>4</v>
       </c>
-      <c r="L105" s="4">
+      <c r="L105">
         <v>3612.7404229612625</v>
       </c>
-      <c r="M105" s="4">
+      <c r="M105">
         <v>4876.5911973899883</v>
       </c>
-      <c r="N105" s="4">
+      <c r="N105">
         <v>4244.6658101756248</v>
       </c>
     </row>
@@ -31539,13 +31913,13 @@
       <c r="K106" s="3">
         <v>8</v>
       </c>
-      <c r="L106" s="4">
+      <c r="L106">
         <v>6568.6596826506357</v>
       </c>
-      <c r="M106" s="4">
+      <c r="M106">
         <v>8558.4679234505275</v>
       </c>
-      <c r="N106" s="4">
+      <c r="N106">
         <v>7563.5638030505825</v>
       </c>
     </row>
@@ -31582,13 +31956,13 @@
       <c r="K107" s="3">
         <v>16</v>
       </c>
-      <c r="L107" s="4">
+      <c r="L107">
         <v>4438.0232260862867</v>
       </c>
-      <c r="M107" s="4">
+      <c r="M107">
         <v>13636.909070896598</v>
       </c>
-      <c r="N107" s="4">
+      <c r="N107">
         <v>9037.4661484914432</v>
       </c>
     </row>
@@ -31625,13 +31999,13 @@
       <c r="K108" s="3">
         <v>32</v>
       </c>
-      <c r="L108" s="4">
+      <c r="L108">
         <v>3223.2295946191352</v>
       </c>
-      <c r="M108" s="4">
+      <c r="M108">
         <v>15133.362040424901</v>
       </c>
-      <c r="N108" s="4">
+      <c r="N108">
         <v>9178.2958175220174</v>
       </c>
     </row>
@@ -31668,13 +32042,13 @@
       <c r="K109" s="3">
         <v>64</v>
       </c>
-      <c r="L109" s="4">
+      <c r="L109">
         <v>3282.1927515595976</v>
       </c>
-      <c r="M109" s="4">
+      <c r="M109">
         <v>15580.51849500221</v>
       </c>
-      <c r="N109" s="4">
+      <c r="N109">
         <v>9431.3556232809042</v>
       </c>
     </row>
@@ -31711,13 +32085,13 @@
       <c r="K110" s="3">
         <v>128</v>
       </c>
-      <c r="L110" s="4">
+      <c r="L110">
         <v>3288.163709660615</v>
       </c>
-      <c r="M110" s="4">
+      <c r="M110">
         <v>15462.413750113148</v>
       </c>
-      <c r="N110" s="4">
+      <c r="N110">
         <v>9375.2887298868827</v>
       </c>
     </row>
@@ -31754,13 +32128,13 @@
       <c r="K111" s="3">
         <v>256</v>
       </c>
-      <c r="L111" s="4">
+      <c r="L111">
         <v>3243.0971845915738</v>
       </c>
-      <c r="M111" s="4">
+      <c r="M111">
         <v>15165.882892997974</v>
       </c>
-      <c r="N111" s="4">
+      <c r="N111">
         <v>9204.4900387947728</v>
       </c>
     </row>
@@ -31797,13 +32171,13 @@
       <c r="K112" s="3">
         <v>512</v>
       </c>
-      <c r="L112" s="4">
+      <c r="L112">
         <v>3263.900874867662</v>
       </c>
-      <c r="M112" s="4">
+      <c r="M112">
         <v>14973.877009866161</v>
       </c>
-      <c r="N112" s="4">
+      <c r="N112">
         <v>9118.8889423669116</v>
       </c>
     </row>
@@ -31840,13 +32214,13 @@
       <c r="K113" s="3">
         <v>1024</v>
       </c>
-      <c r="L113" s="4">
+      <c r="L113">
         <v>3233.272055196278</v>
       </c>
-      <c r="M113" s="4">
+      <c r="M113">
         <v>14148.292896148288</v>
       </c>
-      <c r="N113" s="4">
+      <c r="N113">
         <v>8690.7824756722821</v>
       </c>
     </row>
@@ -31883,13 +32257,13 @@
       <c r="K114" s="3">
         <v>2048</v>
       </c>
-      <c r="L114" s="4">
+      <c r="L114">
         <v>3193.5390171177046</v>
       </c>
-      <c r="M114" s="4">
+      <c r="M114">
         <v>13092.199332543294</v>
       </c>
-      <c r="N114" s="4">
+      <c r="N114">
         <v>8142.8691748304991</v>
       </c>
     </row>
@@ -31926,13 +32300,13 @@
       <c r="K115" s="3">
         <v>4096</v>
       </c>
-      <c r="L115" s="4">
+      <c r="L115">
         <v>3079.8622138927335</v>
       </c>
-      <c r="M115" s="4">
+      <c r="M115">
         <v>11365.472003097888</v>
       </c>
-      <c r="N115" s="4">
+      <c r="N115">
         <v>7222.6671084953095</v>
       </c>
     </row>
@@ -31969,13 +32343,13 @@
       <c r="K116" s="3">
         <v>8192</v>
       </c>
-      <c r="L116" s="4">
+      <c r="L116">
         <v>2818.0683825461874</v>
       </c>
-      <c r="M116" s="4">
+      <c r="M116">
         <v>8935.5481596984228</v>
       </c>
-      <c r="N116" s="4">
+      <c r="N116">
         <v>5876.8082711223042</v>
       </c>
     </row>
@@ -32012,13 +32386,13 @@
       <c r="K117" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L117" s="4">
+      <c r="L117">
         <v>3309.6752720406394</v>
       </c>
-      <c r="M117" s="4">
+      <c r="M117">
         <v>11075.036360012846</v>
       </c>
-      <c r="N117" s="4">
+      <c r="N117">
         <v>7192.3558160267421</v>
       </c>
     </row>

</xml_diff>